<commit_message>
More div in the VBA
</commit_message>
<xml_diff>
--- a/VBA/001 Start To write VBA Codes.xlsx
+++ b/VBA/001 Start To write VBA Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web learning\VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE15F76-8E3F-4A5B-AB58-9103CCA6BC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F385CC7-5C28-4805-AF2D-6030A20D5535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4800" yWindow="-15870" windowWidth="25440" windowHeight="15990" xr2:uid="{5DCA5F7A-398A-4C5A-A02E-FEBB2E5CDE3D}"/>
+    <workbookView xWindow="-915" yWindow="-11145" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{5DCA5F7A-398A-4C5A-A02E-FEBB2E5CDE3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,15 +57,35 @@
 </metadata>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -485,8 +505,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,12 +564,34 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F1F96-33FD-4BDD-8255-98EA0A0E1592}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>MOD(12,5)</f>
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" cellComments="atEnd" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>